<commit_message>
Bug detected (TEST009 the first investment cycle does not test for end of lifecycle)
</commit_message>
<xml_diff>
--- a/Tests - demo of functionality.xlsx
+++ b/Tests - demo of functionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanoord01-my.sharepoint.com/personal/mark_vankoningsveld_vanoord_com/Documents/Software/github/OpenSCSim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="8_{9EF6EF7E-8146-4C87-B37D-99B75FC7BE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{816D038B-BDF3-4AEB-B69D-7FEED37C18F5}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="8_{9EF6EF7E-8146-4C87-B37D-99B75FC7BE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8265707-B5A3-4E2D-91CB-2FDF53A692E3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{2DB130C6-A9F4-4E3E-83A4-36CD790A4E0F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{2DB130C6-A9F4-4E3E-83A4-36CD790A4E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test001" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Test006" sheetId="7" r:id="rId6"/>
     <sheet name="Test007" sheetId="8" r:id="rId7"/>
     <sheet name="Test008" sheetId="1" r:id="rId8"/>
+    <sheet name="Test009" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="36">
   <si>
     <t>capex 1</t>
   </si>
@@ -145,6 +146,12 @@
   </si>
   <si>
     <t>Lifecycle selected exactly 1 economic lifetime + 2 years (not enough to complete new capex cycle)</t>
+  </si>
+  <si>
+    <t>startyear selected to be 10 years after the escalation_base_year. Lifecycle selected exactly 1 economic lifetime + 5 years (enough to complete new capex cycle, and two operational years)</t>
+  </si>
+  <si>
+    <t>********** BUG **********</t>
   </si>
 </sst>
 </file>
@@ -289,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -331,6 +338,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,22 +362,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>17640</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>30238</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>142825</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>114099</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C275CA3-EBC2-B45E-4E99-D1125EB1EC46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{986964C8-27EA-D464-9F02-0D45FFE7545D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -391,8 +400,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12438240" y="2316238"/>
-          <a:ext cx="10577285" cy="5798861"/>
+          <a:off x="12433300" y="2311400"/>
+          <a:ext cx="10591800" cy="5797550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -419,22 +428,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:colOff>139700</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{354AE4C6-01DF-5F05-279C-60AAA76450CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F30318B-DB05-2EB2-2480-9B3002CA2EDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -457,8 +466,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12446000" y="2311400"/>
-          <a:ext cx="10591800" cy="5797550"/>
+          <a:off x="12420600" y="2311400"/>
+          <a:ext cx="10591800" cy="5803900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -485,22 +494,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{210D087D-D7A5-E0C6-1571-BBBC2E86456E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A2594A-9818-F500-759A-F16F5432F9D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -523,7 +532,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12433300" y="2298700"/>
+          <a:off x="12446000" y="2311400"/>
           <a:ext cx="10591800" cy="5803900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -551,22 +560,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5751777-E3A8-13B0-C4C6-3346E3CAD016}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5821B51E-8126-4E42-E4E6-39DE1646F29A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -589,7 +598,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12433300" y="2311400"/>
+          <a:off x="12446000" y="2298700"/>
           <a:ext cx="10591800" cy="5803900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -617,22 +626,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F81EEE-F1B2-B7AD-7D3C-010D5064BB59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C8C539-A782-39DC-C3B4-84C5B73D2A34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -655,8 +664,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12420600" y="2298700"/>
-          <a:ext cx="10591800" cy="5803900"/>
+          <a:off x="12433300" y="2298700"/>
+          <a:ext cx="10591800" cy="5797550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -691,14 +700,14 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{978ECCFE-EBA9-4F8F-82BC-B3D03A46DB32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1896B33F-A96F-A347-4799-D3004FCA6AF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -722,7 +731,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="12433300" y="2298700"/>
-          <a:ext cx="10591800" cy="5803900"/>
+          <a:ext cx="10591800" cy="5797550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -751,20 +760,20 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A86D90C1-8747-6904-D552-50E625664E17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{652D73D9-D149-5677-5720-22CC4BC1CB2F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -787,8 +796,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12420600" y="2298700"/>
-          <a:ext cx="10591800" cy="5803900"/>
+          <a:off x="12420600" y="2311400"/>
+          <a:ext cx="10591800" cy="5797550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -815,22 +824,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>6803</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>9072</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>191860</xdr:colOff>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>107044</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE69796E-CFF0-6135-1FA2-69452B4A2468}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0994AE72-4BF5-D812-B64B-D4CCD64F1635}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -853,8 +862,74 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12427403" y="2295072"/>
-          <a:ext cx="10548257" cy="5812972"/>
+          <a:off x="12433300" y="2311400"/>
+          <a:ext cx="10591800" cy="5797550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{926630A2-A237-6C83-C93D-7D25F4AC9B80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12420600" y="2311400"/>
+          <a:ext cx="10591800" cy="5803900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1176,7 +1251,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1990,7 +2065,7 @@
     <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +2074,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2083,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
@@ -2017,7 +2092,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -2028,7 +2103,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2039,7 +2114,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2050,7 +2125,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
@@ -2061,7 +2136,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
@@ -2072,7 +2147,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
@@ -2081,7 +2156,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2098,7 +2173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <f>C4</f>
         <v>2023</v>
@@ -2113,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
         <f>B11+1</f>
         <v>2024</v>
@@ -2128,7 +2203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
         <f t="shared" ref="B13:B40" si="0">B12+1</f>
         <v>2025</v>
@@ -2143,7 +2218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14" s="14">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -2161,11 +2236,8 @@
         <f>C6+C7</f>
         <v>2026</v>
       </c>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" s="14">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -2181,7 +2253,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" s="14">
         <f t="shared" si="0"/>
         <v>2028</v>
@@ -3198,7 +3270,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B79" s="14">
-        <f t="shared" ref="B79:B81" si="3">B78+1</f>
+        <f t="shared" ref="B79:B80" si="3">B78+1</f>
         <v>2091</v>
       </c>
       <c r="C79" s="14">
@@ -3304,7 +3376,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3998,7 +4070,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4703,7 +4775,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4722,7 +4794,7 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="8"/>
@@ -4734,7 +4806,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
@@ -4754,7 +4826,7 @@
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
         <v>32</v>
       </c>
       <c r="D5" s="8"/>
@@ -5417,7 +5489,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5436,7 +5508,7 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="8"/>
@@ -5448,7 +5520,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
@@ -5468,7 +5540,7 @@
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
         <v>33</v>
       </c>
       <c r="D5" s="8"/>
@@ -6143,7 +6215,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6162,7 +6234,7 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="8"/>
@@ -6174,7 +6246,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
@@ -6194,7 +6266,7 @@
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
         <v>34</v>
       </c>
       <c r="D5" s="8"/>
@@ -6880,8 +6952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D804E2A1-D484-4CA7-872F-CE29998D0066}">
   <dimension ref="B1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6899,7 +6971,7 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="8"/>
@@ -6911,12 +6983,745 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2023</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>35</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2023</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="13">
+        <f>C4</f>
+        <v>2023</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="13">
+        <f>B11+1</f>
+        <v>2024</v>
+      </c>
+      <c r="C12" s="13">
+        <v>2</v>
+      </c>
+      <c r="D12" s="13">
+        <v>2</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="13">
+        <f t="shared" ref="B13:B45" si="0">B12+1</f>
+        <v>2025</v>
+      </c>
+      <c r="C13" s="13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="13">
+        <v>3</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="14">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="C14" s="14">
+        <v>4</v>
+      </c>
+      <c r="D14" s="14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2">
+        <f>C6+C7</f>
+        <v>2026</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="14">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="C15" s="14">
+        <v>5</v>
+      </c>
+      <c r="D15" s="14">
+        <v>5</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="14">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="C16" s="14">
+        <v>6</v>
+      </c>
+      <c r="D16" s="14">
+        <v>6</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="14">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="C17" s="14">
+        <v>7</v>
+      </c>
+      <c r="D17" s="14">
+        <v>7</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="14">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="C18" s="14">
+        <v>8</v>
+      </c>
+      <c r="D18" s="14">
+        <v>8</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="14">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="C19" s="14">
+        <v>9</v>
+      </c>
+      <c r="D19" s="14">
+        <v>9</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="14">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="C20" s="14">
+        <v>10</v>
+      </c>
+      <c r="D20" s="14">
+        <v>10</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="14">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="C21" s="14">
+        <v>11</v>
+      </c>
+      <c r="D21" s="14">
+        <v>11</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="14">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="C22" s="14">
+        <v>12</v>
+      </c>
+      <c r="D22" s="14">
+        <v>12</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="14">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+      <c r="C23" s="14">
+        <v>13</v>
+      </c>
+      <c r="D23" s="14">
+        <v>13</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="14">
+        <f t="shared" si="0"/>
+        <v>2036</v>
+      </c>
+      <c r="C24" s="14">
+        <v>14</v>
+      </c>
+      <c r="D24" s="14">
+        <v>14</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="14">
+        <f t="shared" si="0"/>
+        <v>2037</v>
+      </c>
+      <c r="C25" s="14">
+        <v>15</v>
+      </c>
+      <c r="D25" s="14">
+        <v>15</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="14">
+        <f t="shared" si="0"/>
+        <v>2038</v>
+      </c>
+      <c r="C26" s="14">
+        <v>16</v>
+      </c>
+      <c r="D26" s="14">
+        <v>16</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="14">
+        <f t="shared" si="0"/>
+        <v>2039</v>
+      </c>
+      <c r="C27" s="14">
+        <v>17</v>
+      </c>
+      <c r="D27" s="14">
+        <v>17</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="14">
+        <f t="shared" si="0"/>
+        <v>2040</v>
+      </c>
+      <c r="C28" s="14">
+        <v>18</v>
+      </c>
+      <c r="D28" s="14">
+        <v>18</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="14">
+        <f t="shared" si="0"/>
+        <v>2041</v>
+      </c>
+      <c r="C29" s="14">
+        <v>19</v>
+      </c>
+      <c r="D29" s="14">
+        <v>19</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="14">
+        <f t="shared" si="0"/>
+        <v>2042</v>
+      </c>
+      <c r="C30" s="14">
+        <v>20</v>
+      </c>
+      <c r="D30" s="14">
+        <v>20</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="14">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="C31" s="14">
+        <v>21</v>
+      </c>
+      <c r="D31" s="14">
+        <v>21</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="14">
+        <f t="shared" si="0"/>
+        <v>2044</v>
+      </c>
+      <c r="C32" s="14">
+        <v>22</v>
+      </c>
+      <c r="D32" s="14">
+        <v>22</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B33" s="14">
+        <f t="shared" si="0"/>
+        <v>2045</v>
+      </c>
+      <c r="C33" s="14">
+        <v>23</v>
+      </c>
+      <c r="D33" s="14">
+        <v>23</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B34" s="14">
+        <f t="shared" si="0"/>
+        <v>2046</v>
+      </c>
+      <c r="C34" s="14">
+        <v>24</v>
+      </c>
+      <c r="D34" s="14">
+        <v>24</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B35" s="14">
+        <f t="shared" si="0"/>
+        <v>2047</v>
+      </c>
+      <c r="C35" s="14">
+        <v>25</v>
+      </c>
+      <c r="D35" s="14">
+        <v>25</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B36" s="14">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="C36" s="14">
+        <v>26</v>
+      </c>
+      <c r="D36" s="14">
+        <v>26</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B37" s="14">
+        <f t="shared" si="0"/>
+        <v>2049</v>
+      </c>
+      <c r="C37" s="14">
+        <v>27</v>
+      </c>
+      <c r="D37" s="14">
+        <v>27</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B38" s="14">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="C38" s="14">
+        <v>28</v>
+      </c>
+      <c r="D38" s="14">
+        <v>28</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B39" s="14">
+        <f t="shared" si="0"/>
+        <v>2051</v>
+      </c>
+      <c r="C39" s="14">
+        <v>29</v>
+      </c>
+      <c r="D39" s="14">
+        <v>29</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B40" s="14">
+        <f t="shared" si="0"/>
+        <v>2052</v>
+      </c>
+      <c r="C40" s="14">
+        <v>30</v>
+      </c>
+      <c r="D40" s="14">
+        <v>30</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B41" s="13">
+        <f t="shared" si="0"/>
+        <v>2053</v>
+      </c>
+      <c r="C41" s="13">
+        <v>1</v>
+      </c>
+      <c r="D41" s="13">
+        <v>31</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B42" s="13">
+        <f t="shared" si="0"/>
+        <v>2054</v>
+      </c>
+      <c r="C42" s="13">
+        <v>2</v>
+      </c>
+      <c r="D42" s="13">
+        <v>32</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B43" s="13">
+        <f t="shared" si="0"/>
+        <v>2055</v>
+      </c>
+      <c r="C43" s="13">
+        <v>3</v>
+      </c>
+      <c r="D43" s="13">
+        <v>33</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="2">
+        <f>C6+C7+C8</f>
+        <v>2056</v>
+      </c>
+      <c r="H43" t="s">
+        <v>13</v>
+      </c>
+      <c r="O43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B44" s="14">
+        <f t="shared" si="0"/>
+        <v>2056</v>
+      </c>
+      <c r="C44" s="14">
+        <v>4</v>
+      </c>
+      <c r="D44" s="14">
+        <v>34</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="2">
+        <f>C6+C7+C8</f>
+        <v>2056</v>
+      </c>
+      <c r="H44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B45" s="13">
+        <f t="shared" si="0"/>
+        <v>2057</v>
+      </c>
+      <c r="C45" s="13">
+        <v>5</v>
+      </c>
+      <c r="D45" s="13">
+        <v>35</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="2">
+        <f>C4+C5</f>
+        <v>2058</v>
+      </c>
+      <c r="H45" t="s">
+        <v>20</v>
+      </c>
+      <c r="O45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0EEBA7-2B07-48D1-B52A-FB9959D67994}">
+  <dimension ref="B1:N55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="6" width="33.81640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="C3"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -6927,7 +7732,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
@@ -6938,18 +7743,21 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="8">
-        <v>2023</v>
+        <v>2033</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="N6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
@@ -6960,7 +7768,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
@@ -6971,7 +7779,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
@@ -6980,7 +7788,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -6997,224 +7805,166 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <f>C4</f>
         <v>2023</v>
       </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
       <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
         <f>B11+1</f>
         <v>2024</v>
       </c>
-      <c r="C12" s="13">
-        <v>2</v>
-      </c>
       <c r="D12" s="13">
         <v>2</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
-        <f t="shared" ref="B13:B45" si="0">B12+1</f>
+        <f t="shared" ref="B13:B50" si="0">B12+1</f>
         <v>2025</v>
-      </c>
-      <c r="C13" s="13">
-        <v>3</v>
       </c>
       <c r="D13" s="13">
         <v>3</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" s="14">
         <f t="shared" si="0"/>
         <v>2026</v>
-      </c>
-      <c r="C14" s="14">
-        <v>4</v>
       </c>
       <c r="D14" s="14">
         <v>4</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2">
-        <f>C6+C7</f>
-        <v>2026</v>
-      </c>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B15" s="14">
         <f t="shared" si="0"/>
         <v>2027</v>
-      </c>
-      <c r="C15" s="14">
-        <v>5</v>
       </c>
       <c r="D15" s="14">
         <v>5</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="F15" s="14"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B16" s="14">
         <f t="shared" si="0"/>
         <v>2028</v>
-      </c>
-      <c r="C16" s="14">
-        <v>6</v>
       </c>
       <c r="D16" s="14">
         <v>6</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="F16" s="14"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="14">
         <f t="shared" si="0"/>
         <v>2029</v>
-      </c>
-      <c r="C17" s="14">
-        <v>7</v>
       </c>
       <c r="D17" s="14">
         <v>7</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="F17"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" s="14">
         <f t="shared" si="0"/>
         <v>2030</v>
-      </c>
-      <c r="C18" s="14">
-        <v>8</v>
       </c>
       <c r="D18" s="14">
         <v>8</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="F18" s="14"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="14">
         <f t="shared" si="0"/>
         <v>2031</v>
-      </c>
-      <c r="C19" s="14">
-        <v>9</v>
       </c>
       <c r="D19" s="14">
         <v>9</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="F19" s="14"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="14">
         <f t="shared" si="0"/>
         <v>2032</v>
       </c>
-      <c r="C20" s="14">
-        <v>10</v>
-      </c>
       <c r="D20" s="14">
         <v>10</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="F20" s="14"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="14">
         <f t="shared" si="0"/>
         <v>2033</v>
       </c>
-      <c r="C21" s="14">
-        <v>11</v>
+      <c r="C21" s="13">
+        <v>1</v>
       </c>
       <c r="D21" s="14">
         <v>11</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E21" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="14">
         <f t="shared" si="0"/>
         <v>2034</v>
       </c>
-      <c r="C22" s="14">
-        <v>12</v>
+      <c r="C22" s="13">
+        <v>2</v>
       </c>
       <c r="D22" s="14">
         <v>12</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="E22" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="14"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="14">
         <f t="shared" si="0"/>
         <v>2035</v>
       </c>
-      <c r="C23" s="14">
-        <v>13</v>
+      <c r="C23" s="13">
+        <v>3</v>
       </c>
       <c r="D23" s="14">
         <v>13</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="E23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="14"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" s="14">
         <f t="shared" si="0"/>
         <v>2036</v>
       </c>
       <c r="C24" s="14">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D24" s="14">
         <v>14</v>
@@ -7222,15 +7972,21 @@
       <c r="F24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G24" s="2">
+        <f>C6+C7</f>
+        <v>2036</v>
+      </c>
+      <c r="H24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="14">
         <f t="shared" si="0"/>
         <v>2037</v>
       </c>
       <c r="C25" s="14">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D25" s="14">
         <v>15</v>
@@ -7240,13 +7996,13 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="14">
         <f t="shared" si="0"/>
         <v>2038</v>
       </c>
       <c r="C26" s="14">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D26" s="14">
         <v>16</v>
@@ -7256,13 +8012,13 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="14">
         <f t="shared" si="0"/>
         <v>2039</v>
       </c>
       <c r="C27" s="14">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D27" s="14">
         <v>17</v>
@@ -7272,13 +8028,13 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="14">
         <f t="shared" si="0"/>
         <v>2040</v>
       </c>
       <c r="C28" s="14">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D28" s="14">
         <v>18</v>
@@ -7288,13 +8044,13 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="14">
         <f t="shared" si="0"/>
         <v>2041</v>
       </c>
       <c r="C29" s="14">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D29" s="14">
         <v>19</v>
@@ -7304,13 +8060,13 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="14">
         <f t="shared" si="0"/>
         <v>2042</v>
       </c>
       <c r="C30" s="14">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D30" s="14">
         <v>20</v>
@@ -7320,13 +8076,13 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="14">
         <f t="shared" si="0"/>
         <v>2043</v>
       </c>
       <c r="C31" s="14">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D31" s="14">
         <v>21</v>
@@ -7336,13 +8092,13 @@
       </c>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="14">
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
       <c r="C32" s="14">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D32" s="14">
         <v>22</v>
@@ -7352,13 +8108,13 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="14">
         <f t="shared" si="0"/>
         <v>2045</v>
       </c>
       <c r="C33" s="14">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D33" s="14">
         <v>23</v>
@@ -7368,13 +8124,13 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="14">
         <f t="shared" si="0"/>
         <v>2046</v>
       </c>
       <c r="C34" s="14">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D34" s="14">
         <v>24</v>
@@ -7384,13 +8140,13 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="14">
         <f t="shared" si="0"/>
         <v>2047</v>
       </c>
       <c r="C35" s="14">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D35" s="14">
         <v>25</v>
@@ -7400,13 +8156,13 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" s="14">
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
       <c r="C36" s="14">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D36" s="14">
         <v>26</v>
@@ -7416,13 +8172,13 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" s="14">
         <f t="shared" si="0"/>
         <v>2049</v>
       </c>
       <c r="C37" s="14">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D37" s="14">
         <v>27</v>
@@ -7432,13 +8188,13 @@
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B38" s="14">
         <f t="shared" si="0"/>
         <v>2050</v>
       </c>
       <c r="C38" s="14">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D38" s="14">
         <v>28</v>
@@ -7448,13 +8204,13 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" s="14">
         <f t="shared" si="0"/>
         <v>2051</v>
       </c>
       <c r="C39" s="14">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D39" s="14">
         <v>29</v>
@@ -7464,98 +8220,76 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="14">
         <f t="shared" si="0"/>
         <v>2052</v>
       </c>
       <c r="C40" s="14">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D40" s="14">
         <v>30</v>
       </c>
-      <c r="E40" s="13" t="s">
-        <v>29</v>
-      </c>
       <c r="F40" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B41" s="13">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="14">
         <f t="shared" si="0"/>
         <v>2053</v>
       </c>
-      <c r="C41" s="13">
-        <v>1</v>
-      </c>
-      <c r="D41" s="13">
+      <c r="C41" s="14">
+        <v>21</v>
+      </c>
+      <c r="D41" s="14">
         <v>31</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>0</v>
-      </c>
       <c r="F41" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B42" s="13">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="14">
         <f t="shared" si="0"/>
         <v>2054</v>
       </c>
-      <c r="C42" s="13">
-        <v>2</v>
-      </c>
-      <c r="D42" s="13">
+      <c r="C42" s="14">
+        <v>22</v>
+      </c>
+      <c r="D42" s="14">
         <v>32</v>
       </c>
-      <c r="E42" s="13" t="s">
-        <v>1</v>
-      </c>
       <c r="F42" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B43" s="13">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="14">
         <f t="shared" si="0"/>
         <v>2055</v>
       </c>
-      <c r="C43" s="13">
-        <v>3</v>
-      </c>
-      <c r="D43" s="13">
+      <c r="C43" s="14">
+        <v>23</v>
+      </c>
+      <c r="D43" s="14">
         <v>33</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>2</v>
-      </c>
       <c r="F43" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="2">
-        <f>C6+C7+C8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="14">
+        <f t="shared" si="0"/>
         <v>2056</v>
       </c>
-      <c r="H43" t="s">
-        <v>13</v>
-      </c>
-      <c r="O43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B44" s="14">
-        <f t="shared" si="0"/>
-        <v>2056</v>
-      </c>
       <c r="C44" s="14">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D44" s="14">
         <v>34</v>
@@ -7563,44 +8297,107 @@
       <c r="F44" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G44" s="2">
-        <f>C6+C7+C8</f>
-        <v>2056</v>
-      </c>
-      <c r="H44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B45" s="13">
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B45" s="14">
         <f t="shared" si="0"/>
         <v>2057</v>
       </c>
-      <c r="C45" s="13">
-        <v>5</v>
-      </c>
-      <c r="D45" s="13">
+      <c r="C45" s="14">
+        <v>25</v>
+      </c>
+      <c r="D45" s="14">
         <v>35</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="F45" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46" s="14">
+        <f t="shared" si="0"/>
+        <v>2058</v>
+      </c>
+      <c r="C46" s="14">
+        <v>26</v>
+      </c>
+      <c r="D46" s="14">
+        <v>36</v>
+      </c>
+      <c r="E46" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F46" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G45" s="2">
-        <f>C4+C5</f>
+      <c r="G46" s="2">
+        <f>$C$4+$C$5</f>
         <v>2058</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H46" t="s">
         <v>20</v>
       </c>
-      <c r="O45" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C49"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="F47" s="14"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Drastically simplified code. Seems to work fine now on the 10 testcases
</commit_message>
<xml_diff>
--- a/Tests - demo of functionality.xlsx
+++ b/Tests - demo of functionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanoord01-my.sharepoint.com/personal/mark_vankoningsveld_vanoord_com/Documents/Software/github/OpenSCSim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="8_{9EF6EF7E-8146-4C87-B37D-99B75FC7BE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8265707-B5A3-4E2D-91CB-2FDF53A692E3}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="8_{9EF6EF7E-8146-4C87-B37D-99B75FC7BE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7B389CF-FABA-4B31-BB1D-E9DDCFB66A12}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{2DB130C6-A9F4-4E3E-83A4-36CD790A4E0F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="8" xr2:uid="{2DB130C6-A9F4-4E3E-83A4-36CD790A4E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test001" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Test007" sheetId="8" r:id="rId7"/>
     <sheet name="Test008" sheetId="1" r:id="rId8"/>
     <sheet name="Test009" sheetId="9" r:id="rId9"/>
+    <sheet name="Test010" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="37">
   <si>
     <t>capex 1</t>
   </si>
@@ -151,7 +152,10 @@
     <t>startyear selected to be 10 years after the escalation_base_year. Lifecycle selected exactly 1 economic lifetime + 5 years (enough to complete new capex cycle, and two operational years)</t>
   </si>
   <si>
-    <t>********** BUG **********</t>
+    <t>opex + decomissioning</t>
+  </si>
+  <si>
+    <t>min([startyear+construction_duration+economic_lifetime; escalation_base_year + lifecycle]</t>
   </si>
 </sst>
 </file>
@@ -362,22 +366,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>13230</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>13224</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>149226</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>102124</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{986964C8-27EA-D464-9F02-0D45FFE7545D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74DD169E-5CF9-92D4-818C-A863C61F1405}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -400,8 +404,74 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12433300" y="2311400"/>
-          <a:ext cx="10591800" cy="5797550"/>
+          <a:off x="12461876" y="2235724"/>
+          <a:ext cx="10573808" cy="5645150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>14773</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>243373</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2019AF3-76D3-0968-78F0-2F34202FD68E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12434192" y="2141279"/>
+          <a:ext cx="10521507" cy="5405179"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -428,6 +498,138 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA3B47C-2A0F-82F1-7639-4758332B2779}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12433300" y="2298700"/>
+          <a:ext cx="10591800" cy="5803900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C2D8DB5-D492-F9EA-9D3F-67DBC4A3036E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12433300" y="2311400"/>
+          <a:ext cx="10591800" cy="5803900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
@@ -440,10 +642,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F30318B-DB05-2EB2-2480-9B3002CA2EDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37A8C449-F5A6-E94C-2167-64764AC1A322}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -489,27 +691,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:colOff>139700</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A2594A-9818-F500-759A-F16F5432F9D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B776FE4-B801-5A49-15CE-123D5D81B7F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -532,140 +734,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12446000" y="2311400"/>
+          <a:off x="12420600" y="2286000"/>
           <a:ext cx="10591800" cy="5803900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5821B51E-8126-4E42-E4E6-39DE1646F29A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12446000" y="2298700"/>
-          <a:ext cx="10591800" cy="5803900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C8C539-A782-39DC-C3B4-84C5B73D2A34}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12433300" y="2298700"/>
-          <a:ext cx="10591800" cy="5797550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -692,22 +762,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>139700</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1896B33F-A96F-A347-4799-D3004FCA6AF1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C4D117-C9A4-1E43-98CF-4F4506B6BB22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -730,8 +800,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12433300" y="2298700"/>
-          <a:ext cx="10591800" cy="5797550"/>
+          <a:off x="12420600" y="2216150"/>
+          <a:ext cx="10591800" cy="5613400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -760,20 +830,20 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{652D73D9-D149-5677-5720-22CC4BC1CB2F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F877FA2A-98DE-D607-B521-E1FE87E5032E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -796,8 +866,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12420600" y="2311400"/>
-          <a:ext cx="10591800" cy="5797550"/>
+          <a:off x="12420600" y="2216150"/>
+          <a:ext cx="10591800" cy="5613400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -824,22 +894,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0994AE72-4BF5-D812-B64B-D4CCD64F1635}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E97E8DF7-8ACC-880D-3AEA-8F19D6563024}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -862,8 +932,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12433300" y="2311400"/>
-          <a:ext cx="10591800" cy="5797550"/>
+          <a:off x="12420600" y="2216150"/>
+          <a:ext cx="10591800" cy="5613400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -892,20 +962,20 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{926630A2-A237-6C83-C93D-7D25F4AC9B80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13B3B0B6-62EC-7F2C-A762-3B21EE0A6296}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -928,8 +998,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12420600" y="2311400"/>
-          <a:ext cx="10591800" cy="5803900"/>
+          <a:off x="12420600" y="2216150"/>
+          <a:ext cx="10591800" cy="5613400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1251,7 +1321,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2043,6 +2113,723 @@
       <c r="O50" t="s">
         <v>17</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A2134E-69FC-49C2-BBD7-BAEB5A314DA9}">
+  <dimension ref="B1:O55"/>
+  <sheetViews>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="6" width="33.81640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2023</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>35</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2033</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="13">
+        <f>C4</f>
+        <v>2023</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="13">
+        <f>B11+1</f>
+        <v>2024</v>
+      </c>
+      <c r="D12" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="13">
+        <f t="shared" ref="B13:B55" si="0">B12+1</f>
+        <v>2025</v>
+      </c>
+      <c r="D13" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B14" s="14">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="D14" s="14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="14">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="D15" s="14">
+        <v>5</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="14">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="D16" s="14">
+        <v>6</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="14">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="D17" s="14">
+        <v>7</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="14">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="D18" s="14">
+        <v>8</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="14">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="D19" s="14">
+        <v>9</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="14">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="D20" s="14">
+        <v>10</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="14">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14">
+        <v>11</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="14">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="C22" s="13">
+        <v>2</v>
+      </c>
+      <c r="D22" s="14">
+        <v>12</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="14">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+      <c r="C23" s="13">
+        <v>3</v>
+      </c>
+      <c r="D23" s="14">
+        <v>13</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="14">
+        <f t="shared" si="0"/>
+        <v>2036</v>
+      </c>
+      <c r="C24" s="14">
+        <v>4</v>
+      </c>
+      <c r="D24" s="14">
+        <v>14</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2">
+        <f>C6+C7</f>
+        <v>2036</v>
+      </c>
+      <c r="H24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="14">
+        <f t="shared" si="0"/>
+        <v>2037</v>
+      </c>
+      <c r="C25" s="14">
+        <v>5</v>
+      </c>
+      <c r="D25" s="14">
+        <v>15</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="14">
+        <f t="shared" si="0"/>
+        <v>2038</v>
+      </c>
+      <c r="C26" s="14">
+        <v>6</v>
+      </c>
+      <c r="D26" s="14">
+        <v>16</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="14">
+        <f t="shared" si="0"/>
+        <v>2039</v>
+      </c>
+      <c r="C27" s="14">
+        <v>7</v>
+      </c>
+      <c r="D27" s="14">
+        <v>17</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="14">
+        <f t="shared" si="0"/>
+        <v>2040</v>
+      </c>
+      <c r="C28" s="14">
+        <v>8</v>
+      </c>
+      <c r="D28" s="14">
+        <v>18</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="14">
+        <f t="shared" si="0"/>
+        <v>2041</v>
+      </c>
+      <c r="C29" s="14">
+        <v>9</v>
+      </c>
+      <c r="D29" s="14">
+        <v>19</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="14">
+        <f t="shared" si="0"/>
+        <v>2042</v>
+      </c>
+      <c r="C30" s="14">
+        <v>10</v>
+      </c>
+      <c r="D30" s="14">
+        <v>20</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="14">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="C31" s="14">
+        <v>11</v>
+      </c>
+      <c r="D31" s="14">
+        <v>21</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="14">
+        <f t="shared" si="0"/>
+        <v>2044</v>
+      </c>
+      <c r="C32" s="14">
+        <v>12</v>
+      </c>
+      <c r="D32" s="14">
+        <v>22</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B33" s="14">
+        <f t="shared" si="0"/>
+        <v>2045</v>
+      </c>
+      <c r="C33" s="14">
+        <v>13</v>
+      </c>
+      <c r="D33" s="14">
+        <v>23</v>
+      </c>
+      <c r="E33"/>
+      <c r="F33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B34" s="14">
+        <f t="shared" si="0"/>
+        <v>2046</v>
+      </c>
+      <c r="C34" s="14">
+        <v>14</v>
+      </c>
+      <c r="D34" s="14">
+        <v>24</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B35" s="14">
+        <f t="shared" si="0"/>
+        <v>2047</v>
+      </c>
+      <c r="C35" s="14">
+        <v>15</v>
+      </c>
+      <c r="D35" s="14">
+        <v>25</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B36" s="14">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="C36" s="14">
+        <v>16</v>
+      </c>
+      <c r="D36" s="14">
+        <v>26</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B37" s="14">
+        <f t="shared" si="0"/>
+        <v>2049</v>
+      </c>
+      <c r="C37" s="14">
+        <v>17</v>
+      </c>
+      <c r="D37" s="14">
+        <v>27</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B38" s="14">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="C38" s="14">
+        <v>18</v>
+      </c>
+      <c r="D38" s="14">
+        <v>28</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B39" s="14">
+        <f t="shared" si="0"/>
+        <v>2051</v>
+      </c>
+      <c r="C39" s="14">
+        <v>19</v>
+      </c>
+      <c r="D39" s="14">
+        <v>29</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B40" s="14">
+        <f t="shared" si="0"/>
+        <v>2052</v>
+      </c>
+      <c r="C40" s="14">
+        <v>20</v>
+      </c>
+      <c r="D40" s="14">
+        <v>30</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B41" s="14">
+        <f t="shared" si="0"/>
+        <v>2053</v>
+      </c>
+      <c r="C41" s="14">
+        <v>21</v>
+      </c>
+      <c r="D41" s="14">
+        <v>31</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B42" s="14">
+        <f t="shared" si="0"/>
+        <v>2054</v>
+      </c>
+      <c r="C42" s="14">
+        <v>22</v>
+      </c>
+      <c r="D42" s="14">
+        <v>32</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B43" s="14">
+        <f t="shared" si="0"/>
+        <v>2055</v>
+      </c>
+      <c r="C43" s="14">
+        <v>23</v>
+      </c>
+      <c r="D43" s="14">
+        <v>33</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B44" s="14">
+        <f t="shared" si="0"/>
+        <v>2056</v>
+      </c>
+      <c r="C44" s="14">
+        <v>24</v>
+      </c>
+      <c r="D44" s="14">
+        <v>34</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B45" s="13">
+        <f t="shared" si="0"/>
+        <v>2057</v>
+      </c>
+      <c r="C45" s="13">
+        <v>25</v>
+      </c>
+      <c r="D45" s="13">
+        <v>35</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="2">
+        <f>MIN($C$6+$C$7+$C$8, $C$4+$C$5)</f>
+        <v>2058</v>
+      </c>
+      <c r="H45" t="s">
+        <v>36</v>
+      </c>
+      <c r="O45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="F47" s="14"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2056,7 +2843,7 @@
   <dimension ref="B1:O100"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4070,7 +4857,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4775,7 +5562,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F9"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5489,7 +6276,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6215,7 +7002,7 @@
   <dimension ref="B1:O50"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6953,7 +7740,7 @@
   <dimension ref="B1:O49"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7683,10 +8470,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0EEBA7-2B07-48D1-B52A-FB9959D67994}">
-  <dimension ref="B1:N55"/>
+  <dimension ref="B1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7737,7 +8524,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="8">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -7753,9 +8540,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
-      <c r="N6" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
@@ -7825,7 +8610,7 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
-        <f t="shared" ref="B13:B50" si="0">B12+1</f>
+        <f t="shared" ref="B13:B55" si="0">B12+1</f>
         <v>2025</v>
       </c>
       <c r="D13" s="13">
@@ -8108,7 +8893,7 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="14">
         <f t="shared" si="0"/>
         <v>2045</v>
@@ -8119,12 +8904,13 @@
       <c r="D33" s="14">
         <v>23</v>
       </c>
+      <c r="E33"/>
       <c r="F33" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="14">
         <f t="shared" si="0"/>
         <v>2046</v>
@@ -8140,7 +8926,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" s="14">
         <f t="shared" si="0"/>
         <v>2047</v>
@@ -8156,7 +8942,7 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" s="14">
         <f t="shared" si="0"/>
         <v>2048</v>
@@ -8172,7 +8958,7 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="14">
         <f t="shared" si="0"/>
         <v>2049</v>
@@ -8188,7 +8974,7 @@
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" s="14">
         <f t="shared" si="0"/>
         <v>2050</v>
@@ -8204,7 +8990,7 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" s="14">
         <f t="shared" si="0"/>
         <v>2051</v>
@@ -8220,7 +9006,7 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B40" s="14">
         <f t="shared" si="0"/>
         <v>2052</v>
@@ -8236,7 +9022,7 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" s="14">
         <f t="shared" si="0"/>
         <v>2053</v>
@@ -8252,7 +9038,7 @@
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B42" s="14">
         <f t="shared" si="0"/>
         <v>2054</v>
@@ -8268,7 +9054,7 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" s="14">
         <f t="shared" si="0"/>
         <v>2055</v>
@@ -8283,7 +9069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" s="14">
         <f t="shared" si="0"/>
         <v>2056</v>
@@ -8298,7 +9084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" s="14">
         <f t="shared" si="0"/>
         <v>2057</v>
@@ -8313,7 +9099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" s="14">
         <f t="shared" si="0"/>
         <v>2058</v>
@@ -8324,80 +9110,168 @@
       <c r="D46" s="14">
         <v>36</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="F46" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B47" s="14">
+        <f t="shared" si="0"/>
+        <v>2059</v>
+      </c>
+      <c r="C47" s="14">
+        <v>27</v>
+      </c>
+      <c r="D47" s="14">
+        <v>37</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B48" s="14">
+        <f t="shared" si="0"/>
+        <v>2060</v>
+      </c>
+      <c r="C48" s="14">
+        <v>28</v>
+      </c>
+      <c r="D48" s="14">
+        <v>38</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B49" s="14">
+        <f t="shared" si="0"/>
+        <v>2061</v>
+      </c>
+      <c r="C49" s="14">
+        <v>29</v>
+      </c>
+      <c r="D49" s="14">
+        <v>39</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B50" s="14">
+        <f t="shared" si="0"/>
+        <v>2062</v>
+      </c>
+      <c r="C50" s="14">
+        <v>30</v>
+      </c>
+      <c r="D50" s="14">
+        <v>40</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B51" s="13">
+        <f t="shared" si="0"/>
+        <v>2063</v>
+      </c>
+      <c r="C51" s="13">
+        <v>31</v>
+      </c>
+      <c r="D51" s="13">
+        <v>41</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B52" s="13">
+        <f t="shared" si="0"/>
+        <v>2064</v>
+      </c>
+      <c r="C52" s="13">
+        <v>32</v>
+      </c>
+      <c r="D52" s="13">
+        <v>42</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B53" s="13">
+        <f t="shared" si="0"/>
+        <v>2065</v>
+      </c>
+      <c r="C53" s="13">
+        <v>33</v>
+      </c>
+      <c r="D53" s="13">
+        <v>43</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B54" s="14">
+        <f t="shared" si="0"/>
+        <v>2066</v>
+      </c>
+      <c r="C54" s="14">
+        <v>34</v>
+      </c>
+      <c r="D54" s="14">
+        <v>44</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B55" s="13">
+        <f t="shared" si="0"/>
+        <v>2067</v>
+      </c>
+      <c r="C55" s="13">
+        <v>35</v>
+      </c>
+      <c r="D55" s="13">
+        <v>45</v>
+      </c>
+      <c r="E55" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F46" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="2">
+      <c r="F55" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55" s="2">
         <f>$C$4+$C$5</f>
-        <v>2058</v>
-      </c>
-      <c r="H46" t="s">
+        <v>2068</v>
+      </c>
+      <c r="H55" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="F47" s="14"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="F49" s="14"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="14"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="14"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="14"/>
+      <c r="O55" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>